<commit_message>
boh io non ci capisco piu' niente
</commit_message>
<xml_diff>
--- a/graphs/calibro_non-pretensionata_statico.xlsx
+++ b/graphs/calibro_non-pretensionata_statico.xlsx
@@ -452,16 +452,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>88.23999999999999</v>
+        <v>0.08824</v>
       </c>
       <c r="C2" t="n">
-        <v>162.42</v>
+        <v>1.5933402</v>
       </c>
       <c r="D2" t="n">
         <v>0.02</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06403226187196742</v>
+        <v>0.06403226187196739</v>
       </c>
     </row>
     <row r="3">
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>150.38</v>
+        <v>0.15038</v>
       </c>
       <c r="C3" t="n">
-        <v>142.76</v>
+        <v>1.4004756</v>
       </c>
       <c r="D3" t="n">
         <v>0.02</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06403226187196742</v>
+        <v>0.06403226187196739</v>
       </c>
     </row>
     <row r="4">
@@ -486,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>211.24</v>
+        <v>0.21124</v>
       </c>
       <c r="C4" t="n">
-        <v>122.77</v>
+        <v>1.2043737</v>
       </c>
       <c r="D4" t="n">
         <v>0.02</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06403226187196742</v>
+        <v>0.06403226187196739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>